<commit_message>
update david the prettiest from eliav
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="servers" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="שרתים" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="תא קשר" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="קרונות" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -451,24 +451,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="15.6328125" defaultRowHeight="21.5" customHeight="1"/>
   <cols>
-    <col width="12.6328125" customWidth="1" style="1" min="1" max="2"/>
-    <col width="16.81640625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="1" min="4" max="4"/>
-    <col width="15.1796875" customWidth="1" style="1" min="5" max="5"/>
-    <col width="18.36328125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="12.6328125" customWidth="1" style="1" min="7" max="10"/>
-    <col width="12.6328125" customWidth="1" style="1" min="11" max="16384"/>
+    <col width="21.90625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="21.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>שם פלטפורמה</t>
@@ -499,16 +493,21 @@
           <t>תאריך אחרוון לעדכון</t>
         </is>
       </c>
-    </row>
-    <row r="2">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>אוגדה 36</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="21.5" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>תק"ש שרתים 188</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>משולשת</t>
+          <t>עמדת CCT</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -521,26 +520,26 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+          <t>25/08/2021, 16:03:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="21.5" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>תק"ש שרתים 188</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>ישל"ק 1</t>
+          <t>שרת רדיו CCU</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
@@ -553,26 +552,26 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+          <t>25/08/2021, 16:02:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.5" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>תק"ש שרתים 188</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>ישל"ק 2</t>
+          <t>ידב"ר</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -585,26 +584,26 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+          <t>25/08/2021, 16:02:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="21.5" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>תק"ש שרתים 299</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>ידב"ר</t>
+          <t>עמדת CCT</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -617,26 +616,26 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E5" s="7" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+          <t>25/08/2021, 16:03:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="21.5" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>תק"ש שרתים 299</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>ישל"ק 1</t>
+          <t>שרת רדיו CCU</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -649,26 +648,26 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+          <t>25/08/2021, 16:03:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="21.5" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>תק"ש שרתים 299</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>משולשת</t>
+          <t>ידב"ר</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -681,129 +680,43 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E7" s="7" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>תק"ש מספר 3</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>משולשת</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>6.6.6.6</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>AZ7</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>תק"ש מספר 3</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>ישל"ק 1</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>123.123.123.123</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>AZ8</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>תק"ש מספר 3</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>ישל"ק 2</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>8.8.8.8</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>AZ9</t>
-        </is>
-      </c>
-      <c r="E10" s="8" t="inlineStr">
-        <is>
-          <t>עובד</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>סוף</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>09/08/2021, 12:56:11</t>
-        </is>
-      </c>
+          <t>25/08/2021, 16:02:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="21.5" customHeight="1">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+    </row>
+    <row r="9" ht="21.5" customHeight="1">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+    </row>
+    <row r="10" ht="21.5" customHeight="1">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+    </row>
+    <row r="11" ht="21.5" customHeight="1">
+      <c r="E11" s="1" t="n"/>
+    </row>
+    <row r="12" ht="21.5" customHeight="1">
+      <c r="E12" s="1" t="n"/>
+    </row>
+    <row r="13" ht="21.5" customHeight="1">
+      <c r="E13" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -816,18 +729,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="15.6328125" defaultRowHeight="21.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col width="21.90625" customWidth="1" min="6" max="6"/>
+    <col width="12.6328125" customWidth="1" style="1" min="1" max="2"/>
+    <col width="16.81640625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="1" min="4" max="4"/>
+    <col width="15.1796875" customWidth="1" style="1" min="5" max="5"/>
+    <col width="18.36328125" customWidth="1" style="1" min="6" max="6"/>
+    <col width="12.6328125" customWidth="1" style="1" min="7" max="12"/>
+    <col width="12.6328125" customWidth="1" style="1" min="13" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.5" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>שם פלטפורמה</t>
@@ -859,15 +778,15 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="21.5" customHeight="1">
+    <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>תק"ש שרתים 188</t>
+          <t>תק"ש מספר 1</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>עמדת CCT</t>
+          <t>משולשת</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -880,26 +799,26 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>09/08/2021, 14:07:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="21.5" customHeight="1">
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>תק"ש שרתים 188</t>
+          <t>תק"ש מספר 1</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>שרת רדיו CCU</t>
+          <t>ישל"ק 1</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
@@ -912,26 +831,26 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
+      <c r="E3" s="9" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>09/08/2021, 14:07:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="21.5" customHeight="1">
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>תק"ש שרתים 188</t>
+          <t>תק"ש מספר 1</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>ידב"ר</t>
+          <t>ישל"ק 2</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
@@ -944,26 +863,26 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="7" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
+      <c r="E4" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>09/08/2021, 14:07:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="21.5" customHeight="1">
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>תק"ש שרתים 299</t>
+          <t>תק"ש מספר 2</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>עמדת CCT</t>
+          <t>ידב"ר</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
@@ -976,26 +895,26 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="E5" s="9" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>09/08/2021, 14:07:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="21.5" customHeight="1">
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>תק"ש שרתים 299</t>
+          <t>תק"ש מספר 2</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>שרת רדיו CCU</t>
+          <t>ישל"ק 1</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
@@ -1008,26 +927,26 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>09/08/2021, 14:07:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="21.5" customHeight="1">
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>תק"ש שרתים 299</t>
+          <t>תק"ש מספר 2</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>ידב"ר</t>
+          <t>משולשת</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
@@ -1040,43 +959,129 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
+      <c r="E7" s="9" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>09/08/2021, 14:07:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="21.5" customHeight="1">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="n"/>
-    </row>
-    <row r="9" ht="21.5" customHeight="1">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
-    </row>
-    <row r="10" ht="21.5" customHeight="1">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
-      <c r="D10" s="1" t="n"/>
-    </row>
-    <row r="11" ht="21.5" customHeight="1">
-      <c r="E11" s="1" t="n"/>
-    </row>
-    <row r="12" ht="21.5" customHeight="1">
-      <c r="E12" s="1" t="n"/>
-    </row>
-    <row r="13" ht="21.5" customHeight="1">
-      <c r="E13" s="1" t="n"/>
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 3</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>AZ7</t>
+        </is>
+      </c>
+      <c r="E8" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 3</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>123.123.123.123</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>AZ8</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 3</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>AZ9</t>
+        </is>
+      </c>
+      <c r="E10" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>סוף</t>
+        </is>
+      </c>
+      <c r="E11" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>25/08/2021, 16:03:00</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1091,7 +1096,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
@@ -1099,8 +1104,8 @@
   <cols>
     <col width="11.1796875" customWidth="1" style="1" min="1" max="5"/>
     <col width="16.90625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="11.1796875" customWidth="1" style="1" min="7" max="7"/>
-    <col width="11.1796875" customWidth="1" style="1" min="8" max="16384"/>
+    <col width="11.1796875" customWidth="1" style="1" min="7" max="9"/>
+    <col width="11.1796875" customWidth="1" style="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.5" customHeight="1">
@@ -1163,7 +1168,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1200,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1232,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:13</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1264,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1296,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1323,7 +1328,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1355,7 +1360,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1380,14 +1385,14 @@
           <t>ZN08</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
-        <is>
-          <t>עובד</t>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1424,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:11</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1456,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1488,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:12</t>
         </is>
       </c>
     </row>
@@ -1515,7 +1520,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1552,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1584,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1616,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1643,7 +1648,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:14</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1680,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1712,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1744,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1776,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1803,7 +1808,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1835,7 +1840,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1867,7 +1872,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1899,7 +1904,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>
@@ -1931,7 +1936,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>09/08/2021, 12:56:19</t>
+          <t>25/08/2021, 16:03:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added a update state for the UI that refresh each frame
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="שרתים" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,12 +18,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -453,7 +459,7 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -527,7 +533,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:10</t>
+          <t>26/08/2021, 13:52:51</t>
         </is>
       </c>
     </row>
@@ -559,7 +565,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:02:57</t>
+          <t>26/08/2021, 13:52:51</t>
         </is>
       </c>
     </row>
@@ -591,7 +597,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:02:57</t>
+          <t>26/08/2021, 13:52:51</t>
         </is>
       </c>
     </row>
@@ -623,7 +629,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:07</t>
+          <t>26/08/2021, 13:52:51</t>
         </is>
       </c>
     </row>
@@ -655,7 +661,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:09</t>
+          <t>26/08/2021, 13:52:51</t>
         </is>
       </c>
     </row>
@@ -687,7 +693,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:02:57</t>
+          <t>26/08/2021, 13:52:51</t>
         </is>
       </c>
     </row>
@@ -729,10 +735,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="14.5"/>
@@ -742,8 +748,8 @@
     <col width="14.54296875" customWidth="1" style="1" min="4" max="4"/>
     <col width="15.1796875" customWidth="1" style="1" min="5" max="5"/>
     <col width="18.36328125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="12.6328125" customWidth="1" style="1" min="7" max="12"/>
-    <col width="12.6328125" customWidth="1" style="1" min="13" max="16384"/>
+    <col width="12.6328125" customWidth="1" style="1" min="7" max="13"/>
+    <col width="12.6328125" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -806,7 +812,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -838,7 +844,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -870,7 +876,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -902,7 +908,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -934,7 +940,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -966,7 +972,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -991,14 +997,14 @@
           <t>AZ7</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="4" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:33:21</t>
         </is>
       </c>
     </row>
@@ -1023,14 +1029,14 @@
           <t>AZ8</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:33:21</t>
         </is>
       </c>
     </row>
@@ -1055,31 +1061,127 @@
           <t>AZ9</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:00</t>
+          <t>26/08/2021, 13:33:21</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>תק"ש מספר 4</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>AZ7</t>
+        </is>
+      </c>
+      <c r="E11" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>26/08/2021, 13:52:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 4</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>AZ8</t>
+        </is>
+      </c>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>26/08/2021, 13:52:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 4</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>AZ9</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>26/08/2021, 13:52:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
           <t>סוף</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>25/08/2021, 16:03:00</t>
+      <c r="E14" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>26/08/2021, 13:52:59</t>
         </is>
       </c>
     </row>
@@ -1104,8 +1206,8 @@
   <cols>
     <col width="11.1796875" customWidth="1" style="1" min="1" max="5"/>
     <col width="16.90625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="11.1796875" customWidth="1" style="1" min="7" max="9"/>
-    <col width="11.1796875" customWidth="1" style="1" min="10" max="16384"/>
+    <col width="11.1796875" customWidth="1" style="1" min="7" max="10"/>
+    <col width="11.1796875" customWidth="1" style="1" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.5" customHeight="1">
@@ -1168,7 +1270,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1302,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1334,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:13</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1366,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1398,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1430,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1462,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1385,14 +1487,14 @@
           <t>ZN08</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
+      <c r="E9" s="8" t="inlineStr">
+        <is>
+          <t>עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1526,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:11</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1558,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1590,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:12</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1622,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1552,7 +1654,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1584,7 +1686,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1616,7 +1718,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1750,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:14</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1782,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1712,7 +1814,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1744,7 +1846,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1878,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1808,7 +1910,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1942,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1872,7 +1974,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1904,7 +2006,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>
@@ -1936,7 +2038,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>25/08/2021, 16:03:01</t>
+          <t>26/08/2021, 13:52:41</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added a setting window when click on "הגדרות" button
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="שרתים" sheetId="1" state="visible" r:id="rId1"/>
@@ -33,7 +33,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -63,10 +63,20 @@
     <fill>
       <gradientFill type="linear">
         <stop position="0">
-          <color rgb="0080ff72"/>
+          <color rgb="FF80FF72"/>
         </stop>
         <stop position="1">
-          <color rgb="007ee8fa"/>
+          <color rgb="FF7EE8FA"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear">
+        <stop position="0">
+          <color rgb="FFFC9842"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFE5F75"/>
         </stop>
       </gradientFill>
     </fill>
@@ -77,6 +87,16 @@
         </stop>
         <stop position="1">
           <color rgb="00fe5f75"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear">
+        <stop position="0">
+          <color rgb="0080ff72"/>
+        </stop>
+        <stop position="1">
+          <color rgb="007ee8fa"/>
         </stop>
       </gradientFill>
     </fill>
@@ -93,15 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -114,6 +128,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,14 +548,14 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>עובד</t>
+      <c r="E2" s="8" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:51</t>
+          <t>03/10/2021, 15:52:46</t>
         </is>
       </c>
     </row>
@@ -558,14 +580,14 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
+      <c r="E3" s="8" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:51</t>
+          <t>03/10/2021, 15:52:46</t>
         </is>
       </c>
     </row>
@@ -590,14 +612,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>עובד</t>
+      <c r="E4" s="8" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:51</t>
+          <t>03/10/2021, 15:52:46</t>
         </is>
       </c>
     </row>
@@ -622,14 +644,14 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="E5" s="8" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:51</t>
+          <t>03/10/2021, 15:52:46</t>
         </is>
       </c>
     </row>
@@ -654,14 +676,14 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>עובד</t>
+      <c r="E6" s="8" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:51</t>
+          <t>03/10/2021, 15:52:46</t>
         </is>
       </c>
     </row>
@@ -686,14 +708,14 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
+      <c r="E7" s="8" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:51</t>
+          <t>03/10/2021, 15:52:46</t>
         </is>
       </c>
     </row>
@@ -737,8 +759,8 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="14.5"/>
@@ -748,8 +770,8 @@
     <col width="14.54296875" customWidth="1" style="1" min="4" max="4"/>
     <col width="15.1796875" customWidth="1" style="1" min="5" max="5"/>
     <col width="18.36328125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="12.6328125" customWidth="1" style="1" min="7" max="13"/>
-    <col width="12.6328125" customWidth="1" style="1" min="14" max="16384"/>
+    <col width="12.6328125" customWidth="1" style="1" min="7" max="15"/>
+    <col width="12.6328125" customWidth="1" style="1" min="16" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -805,14 +827,14 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E2" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -844,7 +866,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -869,14 +891,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
-        <is>
-          <t>עובד</t>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -908,7 +930,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -933,14 +955,14 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E6" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -972,7 +994,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -997,7 +1019,7 @@
           <t>AZ7</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -1029,7 +1051,7 @@
           <t>AZ8</t>
         </is>
       </c>
-      <c r="E9" s="5" t="inlineStr">
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
@@ -1061,7 +1083,7 @@
           <t>AZ9</t>
         </is>
       </c>
-      <c r="E10" s="4" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -1093,14 +1115,14 @@
           <t>AZ7</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="E11" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -1125,14 +1147,14 @@
           <t>AZ8</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -1157,14 +1179,14 @@
           <t>AZ9</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="E13" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1203,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:59</t>
+          <t>03/10/2021, 15:52:39</t>
         </is>
       </c>
     </row>
@@ -1196,18 +1218,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.1796875" defaultRowHeight="26.5" customHeight="1"/>
   <cols>
     <col width="11.1796875" customWidth="1" style="1" min="1" max="5"/>
     <col width="16.90625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="11.1796875" customWidth="1" style="1" min="7" max="10"/>
-    <col width="11.1796875" customWidth="1" style="1" min="11" max="16384"/>
+    <col width="11.1796875" customWidth="1" style="1" min="7" max="12"/>
+    <col width="11.1796875" customWidth="1" style="1" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.5" customHeight="1">
@@ -1263,14 +1285,14 @@
           <t>ZN01</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E2" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1324,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1356,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1388,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1420,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1452,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1484,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1487,14 +1509,14 @@
           <t>ZN08</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1548,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1580,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1612,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1644,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1654,7 +1676,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1708,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1711,14 +1733,14 @@
           <t>ZN15</t>
         </is>
       </c>
-      <c r="E16" s="8" t="inlineStr">
+      <c r="E16" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1772,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1782,7 +1804,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1814,7 +1836,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1868,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1878,7 +1900,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1932,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1935,14 +1957,14 @@
           <t>ZN22</t>
         </is>
       </c>
-      <c r="E23" s="8" t="inlineStr">
+      <c r="E23" s="10" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -1974,7 +1996,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2028,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2060,199 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:52:41</t>
+          <t>03/10/2021, 15:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="26.5" customHeight="1">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>קרון ד</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.12</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>ZN26</t>
+        </is>
+      </c>
+      <c r="E27" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>03/10/2021, 15:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="26.5" customHeight="1">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>קרון ד</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>ZN27</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>03/10/2021, 15:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="26.5" customHeight="1">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>קרון ד</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.14</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>ZN28</t>
+        </is>
+      </c>
+      <c r="E29" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>03/10/2021, 15:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="26.5" customHeight="1">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>קרון ד</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.15</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>ZN29</t>
+        </is>
+      </c>
+      <c r="E30" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>03/10/2021, 15:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="26.5" customHeight="1">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>קרון ד</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.16</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>ZN30</t>
+        </is>
+      </c>
+      <c r="E31" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>03/10/2021, 15:52:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="26.5" customHeight="1">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>קרון ד</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.17</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>ZN31</t>
+        </is>
+      </c>
+      <c r="E32" s="9" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>03/10/2021, 15:52:41</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
before adding a new screen to the ui
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="שרתים" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="תא קשר" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="קרונות" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="לבדוק בנוסף" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -33,7 +34,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
@@ -47,6 +48,16 @@
         </stop>
         <stop position="1">
           <color rgb="FF7EE8FA"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear">
+        <stop position="0">
+          <color rgb="FFFC9842"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFE5F75"/>
         </stop>
       </gradientFill>
     </fill>
@@ -83,10 +94,10 @@
     <fill>
       <gradientFill type="linear">
         <stop position="0">
-          <color rgb="00fc9842"/>
+          <color rgb="FF80FF72"/>
         </stop>
         <stop position="1">
-          <color rgb="00fe5f75"/>
+          <color rgb="FF7EE8FA"/>
         </stop>
       </gradientFill>
     </fill>
@@ -97,6 +108,16 @@
         </stop>
         <stop position="1">
           <color rgb="007ee8fa"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear">
+        <stop position="0">
+          <color rgb="00fc9842"/>
+        </stop>
+        <stop position="1">
+          <color rgb="00fe5f75"/>
         </stop>
       </gradientFill>
     </fill>
@@ -113,29 +134,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,14 +571,14 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:46</t>
+          <t>17/10/2021, 16:43:48</t>
         </is>
       </c>
     </row>
@@ -580,14 +603,14 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="11" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:46</t>
+          <t>17/10/2021, 16:43:48</t>
         </is>
       </c>
     </row>
@@ -612,14 +635,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="E4" s="11" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:46</t>
+          <t>17/10/2021, 16:43:48</t>
         </is>
       </c>
     </row>
@@ -644,14 +667,14 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="E5" s="11" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:46</t>
+          <t>17/10/2021, 16:43:48</t>
         </is>
       </c>
     </row>
@@ -676,14 +699,14 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
+      <c r="E6" s="10" t="inlineStr">
+        <is>
+          <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:46</t>
+          <t>17/10/2021, 16:43:48</t>
         </is>
       </c>
     </row>
@@ -708,14 +731,14 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="E7" s="11" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:46</t>
+          <t>17/10/2021, 16:43:48</t>
         </is>
       </c>
     </row>
@@ -760,7 +783,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A1" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="14.5"/>
@@ -770,8 +793,8 @@
     <col width="14.54296875" customWidth="1" style="1" min="4" max="4"/>
     <col width="15.1796875" customWidth="1" style="1" min="5" max="5"/>
     <col width="18.36328125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="12.6328125" customWidth="1" style="1" min="7" max="15"/>
-    <col width="12.6328125" customWidth="1" style="1" min="16" max="16384"/>
+    <col width="12.6328125" customWidth="1" style="1" min="7" max="17"/>
+    <col width="12.6328125" customWidth="1" style="1" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -827,14 +850,14 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -859,14 +882,14 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -891,14 +914,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="E4" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -923,14 +946,14 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -955,14 +978,14 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="10" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -987,14 +1010,14 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -1115,14 +1138,14 @@
           <t>AZ7</t>
         </is>
       </c>
-      <c r="E11" s="10" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -1147,14 +1170,14 @@
           <t>AZ8</t>
         </is>
       </c>
-      <c r="E12" s="10" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -1179,14 +1202,14 @@
           <t>AZ9</t>
         </is>
       </c>
-      <c r="E13" s="10" t="inlineStr">
+      <c r="E13" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -1196,14 +1219,14 @@
           <t>סוף</t>
         </is>
       </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="E14" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:39</t>
+          <t>17/10/2021, 16:43:40</t>
         </is>
       </c>
     </row>
@@ -1220,7 +1243,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -1228,8 +1251,8 @@
   <cols>
     <col width="11.1796875" customWidth="1" style="1" min="1" max="5"/>
     <col width="16.90625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="11.1796875" customWidth="1" style="1" min="7" max="12"/>
-    <col width="11.1796875" customWidth="1" style="1" min="13" max="16384"/>
+    <col width="11.1796875" customWidth="1" style="1" min="7" max="14"/>
+    <col width="11.1796875" customWidth="1" style="1" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.5" customHeight="1">
@@ -1285,14 +1308,14 @@
           <t>ZN01</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1317,14 +1340,14 @@
           <t>ZN02</t>
         </is>
       </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="E3" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1349,14 +1372,14 @@
           <t>ZN03</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="E4" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1381,14 +1404,14 @@
           <t>ZN04</t>
         </is>
       </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="E5" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1413,14 +1436,14 @@
           <t>ZN05</t>
         </is>
       </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="E6" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1445,14 +1468,14 @@
           <t>ZN06</t>
         </is>
       </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="E7" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1477,14 +1500,14 @@
           <t>ZN07</t>
         </is>
       </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="E8" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1509,14 +1532,14 @@
           <t>ZN08</t>
         </is>
       </c>
-      <c r="E9" s="10" t="inlineStr">
+      <c r="E9" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1541,14 +1564,14 @@
           <t>ZN09</t>
         </is>
       </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="E10" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1573,14 +1596,14 @@
           <t>ZN10</t>
         </is>
       </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="E11" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1605,14 +1628,14 @@
           <t>ZN11</t>
         </is>
       </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="E12" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1637,14 +1660,14 @@
           <t>ZN12</t>
         </is>
       </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="E13" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1669,14 +1692,14 @@
           <t>ZN13</t>
         </is>
       </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="E14" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1701,14 +1724,14 @@
           <t>ZN14</t>
         </is>
       </c>
-      <c r="E15" s="9" t="inlineStr">
+      <c r="E15" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1733,14 +1756,14 @@
           <t>ZN15</t>
         </is>
       </c>
-      <c r="E16" s="10" t="inlineStr">
+      <c r="E16" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1765,14 +1788,14 @@
           <t>ZN16</t>
         </is>
       </c>
-      <c r="E17" s="9" t="inlineStr">
+      <c r="E17" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1797,14 +1820,14 @@
           <t>ZN17</t>
         </is>
       </c>
-      <c r="E18" s="9" t="inlineStr">
+      <c r="E18" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1829,14 +1852,14 @@
           <t>ZN18</t>
         </is>
       </c>
-      <c r="E19" s="9" t="inlineStr">
+      <c r="E19" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1861,14 +1884,14 @@
           <t>ZN19</t>
         </is>
       </c>
-      <c r="E20" s="9" t="inlineStr">
+      <c r="E20" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1893,14 +1916,14 @@
           <t>ZN20</t>
         </is>
       </c>
-      <c r="E21" s="9" t="inlineStr">
+      <c r="E21" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1925,14 +1948,14 @@
           <t>ZN21</t>
         </is>
       </c>
-      <c r="E22" s="9" t="inlineStr">
+      <c r="E22" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1957,14 +1980,14 @@
           <t>ZN22</t>
         </is>
       </c>
-      <c r="E23" s="10" t="inlineStr">
+      <c r="E23" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -1989,14 +2012,14 @@
           <t>ZN23</t>
         </is>
       </c>
-      <c r="E24" s="9" t="inlineStr">
+      <c r="E24" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2021,14 +2044,14 @@
           <t>ZN24</t>
         </is>
       </c>
-      <c r="E25" s="9" t="inlineStr">
+      <c r="E25" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2053,14 +2076,14 @@
           <t>ZN25</t>
         </is>
       </c>
-      <c r="E26" s="9" t="inlineStr">
+      <c r="E26" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2085,14 +2108,14 @@
           <t>ZN26</t>
         </is>
       </c>
-      <c r="E27" s="9" t="inlineStr">
+      <c r="E27" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2117,14 +2140,14 @@
           <t>ZN27</t>
         </is>
       </c>
-      <c r="E28" s="10" t="inlineStr">
+      <c r="E28" s="12" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2149,14 +2172,14 @@
           <t>ZN28</t>
         </is>
       </c>
-      <c r="E29" s="9" t="inlineStr">
+      <c r="E29" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2181,14 +2204,14 @@
           <t>ZN29</t>
         </is>
       </c>
-      <c r="E30" s="9" t="inlineStr">
+      <c r="E30" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2213,14 +2236,14 @@
           <t>ZN30</t>
         </is>
       </c>
-      <c r="E31" s="9" t="inlineStr">
+      <c r="E31" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>
@@ -2245,14 +2268,580 @@
           <t>ZN31</t>
         </is>
       </c>
-      <c r="E32" s="9" t="inlineStr">
+      <c r="E32" s="13" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>03/10/2021, 15:52:41</t>
+          <t>17/10/2021, 16:43:42</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="14.7265625" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>שם פלטפורמה</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>סוג מכשיר</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hostname</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>תאריך אחרוון לעדכון</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>AZ1</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>12.12.2.12</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>AZ2</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>AZ1</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>12.12.2.12</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>AZ2</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>AZ1</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>12.12.2.12</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>AZ2</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E10" s="5" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:38:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>AZ1</t>
+        </is>
+      </c>
+      <c r="E11" s="12" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>17/10/2021, 16:43:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>12.12.2.12</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>AZ2</t>
+        </is>
+      </c>
+      <c r="E12" s="13" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>17/10/2021, 16:43:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 1</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:47:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 2</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:47:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 2</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:47:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 2</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>05/10/2021, 15:47:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 2</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>AZ3</t>
+        </is>
+      </c>
+      <c r="E17" s="13" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>17/10/2021, 16:43:42</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
start to build the json database
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="שרתים" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,29 +27,13 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <gradientFill type="linear">
-        <stop position="0">
-          <color rgb="FF80FF72"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF7EE8FA"/>
-        </stop>
-      </gradientFill>
     </fill>
     <fill>
       <gradientFill type="linear">
@@ -64,10 +48,10 @@
     <fill>
       <gradientFill type="linear">
         <stop position="0">
-          <color rgb="FFFC9842"/>
+          <color rgb="FF80FF72"/>
         </stop>
         <stop position="1">
-          <color rgb="FFFE5F75"/>
+          <color rgb="FF7EE8FA"/>
         </stop>
       </gradientFill>
     </fill>
@@ -134,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -142,23 +126,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,14 +554,14 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E2" s="9" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:48</t>
+          <t>20/10/2021, 17:10:02</t>
         </is>
       </c>
     </row>
@@ -603,14 +586,14 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="11" t="inlineStr">
+      <c r="E3" s="10" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:48</t>
+          <t>20/10/2021, 17:10:02</t>
         </is>
       </c>
     </row>
@@ -635,14 +618,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="10" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:48</t>
+          <t>20/10/2021, 17:10:02</t>
         </is>
       </c>
     </row>
@@ -667,14 +650,14 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="11" t="inlineStr">
+      <c r="E5" s="10" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:48</t>
+          <t>20/10/2021, 17:10:02</t>
         </is>
       </c>
     </row>
@@ -699,14 +682,14 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="10" t="inlineStr">
+      <c r="E6" s="9" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:48</t>
+          <t>20/10/2021, 17:10:02</t>
         </is>
       </c>
     </row>
@@ -731,14 +714,14 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
+      <c r="E7" s="10" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:48</t>
+          <t>20/10/2021, 17:10:02</t>
         </is>
       </c>
     </row>
@@ -780,10 +763,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="14.5"/>
@@ -793,8 +776,8 @@
     <col width="14.54296875" customWidth="1" style="1" min="4" max="4"/>
     <col width="15.1796875" customWidth="1" style="1" min="5" max="5"/>
     <col width="18.36328125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="12.6328125" customWidth="1" style="1" min="7" max="17"/>
-    <col width="12.6328125" customWidth="1" style="1" min="18" max="16384"/>
+    <col width="12.6328125" customWidth="1" style="1" min="7" max="19"/>
+    <col width="12.6328125" customWidth="1" style="1" min="20" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -850,14 +833,14 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="12" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -882,14 +865,14 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="13" t="inlineStr">
+      <c r="E3" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -914,14 +897,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="13" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -946,14 +929,14 @@
           <t>AZ4</t>
         </is>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -978,14 +961,14 @@
           <t>AZ5</t>
         </is>
       </c>
-      <c r="E6" s="12" t="inlineStr">
+      <c r="E6" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1010,14 +993,14 @@
           <t>AZ6</t>
         </is>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1042,14 +1025,14 @@
           <t>AZ7</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>עובד</t>
+      <c r="E8" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:33:21</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1074,14 +1057,14 @@
           <t>AZ8</t>
         </is>
       </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="E9" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:33:21</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1106,14 +1089,14 @@
           <t>AZ9</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E10" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>26/08/2021, 13:33:21</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1135,17 +1118,17 @@
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>AZ7</t>
-        </is>
-      </c>
-      <c r="E11" s="12" t="inlineStr">
+          <t>AZ10</t>
+        </is>
+      </c>
+      <c r="E11" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1167,17 +1150,17 @@
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
-          <t>AZ8</t>
-        </is>
-      </c>
-      <c r="E12" s="12" t="inlineStr">
+          <t>AZ11</t>
+        </is>
+      </c>
+      <c r="E12" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
@@ -1199,34 +1182,322 @@
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>AZ9</t>
-        </is>
-      </c>
-      <c r="E13" s="12" t="inlineStr">
+          <t>AZ12</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:40</t>
+          <t>20/10/2021, 17:09:54</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
+          <t>תק"ש מספר 5</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>AZ13</t>
+        </is>
+      </c>
+      <c r="E14" s="11" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 5</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>12.12.2.12</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>AZ14</t>
+        </is>
+      </c>
+      <c r="E15" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 5</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>AZ15</t>
+        </is>
+      </c>
+      <c r="E16" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 6</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>ידב"ר</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>123.123.123.123</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>AZ16</t>
+        </is>
+      </c>
+      <c r="E17" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 6</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>AZ17</t>
+        </is>
+      </c>
+      <c r="E18" s="11" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 6</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>12.12.2.12</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>AZ18</t>
+        </is>
+      </c>
+      <c r="E19" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 7</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>משולשת</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>6.6.6.6</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>AZ19</t>
+        </is>
+      </c>
+      <c r="E20" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 7</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 1</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>123.123.123.123</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>AZ20</t>
+        </is>
+      </c>
+      <c r="E21" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>תק"ש מספר 7</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>ישל"ק 2</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>AZ21</t>
+        </is>
+      </c>
+      <c r="E22" s="11" t="inlineStr">
+        <is>
+          <t>עובד</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>20/10/2021, 17:09:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
           <t>סוף</t>
         </is>
       </c>
-      <c r="E14" s="13" t="inlineStr">
-        <is>
-          <t>לא עובד</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>17/10/2021, 16:43:40</t>
+      <c r="E23" s="12" t="inlineStr">
+        <is>
+          <t>לא עובד</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>18/10/2021, 10:24:59</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1514,7 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -1251,8 +1522,8 @@
   <cols>
     <col width="11.1796875" customWidth="1" style="1" min="1" max="5"/>
     <col width="16.90625" customWidth="1" style="1" min="6" max="6"/>
-    <col width="11.1796875" customWidth="1" style="1" min="7" max="14"/>
-    <col width="11.1796875" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="11.1796875" customWidth="1" style="1" min="7" max="16"/>
+    <col width="11.1796875" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.5" customHeight="1">
@@ -1308,14 +1579,14 @@
           <t>ZN01</t>
         </is>
       </c>
-      <c r="E2" s="12" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1340,14 +1611,14 @@
           <t>ZN02</t>
         </is>
       </c>
-      <c r="E3" s="13" t="inlineStr">
+      <c r="E3" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1372,14 +1643,14 @@
           <t>ZN03</t>
         </is>
       </c>
-      <c r="E4" s="13" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1404,14 +1675,14 @@
           <t>ZN04</t>
         </is>
       </c>
-      <c r="E5" s="13" t="inlineStr">
+      <c r="E5" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1436,14 +1707,14 @@
           <t>ZN05</t>
         </is>
       </c>
-      <c r="E6" s="13" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1468,14 +1739,14 @@
           <t>ZN06</t>
         </is>
       </c>
-      <c r="E7" s="13" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1500,14 +1771,14 @@
           <t>ZN07</t>
         </is>
       </c>
-      <c r="E8" s="13" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1532,14 +1803,14 @@
           <t>ZN08</t>
         </is>
       </c>
-      <c r="E9" s="12" t="inlineStr">
+      <c r="E9" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1564,14 +1835,14 @@
           <t>ZN09</t>
         </is>
       </c>
-      <c r="E10" s="13" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1596,14 +1867,14 @@
           <t>ZN10</t>
         </is>
       </c>
-      <c r="E11" s="13" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1628,14 +1899,14 @@
           <t>ZN11</t>
         </is>
       </c>
-      <c r="E12" s="13" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1660,14 +1931,14 @@
           <t>ZN12</t>
         </is>
       </c>
-      <c r="E13" s="13" t="inlineStr">
+      <c r="E13" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1692,14 +1963,14 @@
           <t>ZN13</t>
         </is>
       </c>
-      <c r="E14" s="13" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1724,14 +1995,14 @@
           <t>ZN14</t>
         </is>
       </c>
-      <c r="E15" s="13" t="inlineStr">
+      <c r="E15" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1756,14 +2027,14 @@
           <t>ZN15</t>
         </is>
       </c>
-      <c r="E16" s="12" t="inlineStr">
+      <c r="E16" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1788,14 +2059,14 @@
           <t>ZN16</t>
         </is>
       </c>
-      <c r="E17" s="13" t="inlineStr">
+      <c r="E17" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1820,14 +2091,14 @@
           <t>ZN17</t>
         </is>
       </c>
-      <c r="E18" s="13" t="inlineStr">
+      <c r="E18" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1852,14 +2123,14 @@
           <t>ZN18</t>
         </is>
       </c>
-      <c r="E19" s="13" t="inlineStr">
+      <c r="E19" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1884,14 +2155,14 @@
           <t>ZN19</t>
         </is>
       </c>
-      <c r="E20" s="13" t="inlineStr">
+      <c r="E20" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1916,14 +2187,14 @@
           <t>ZN20</t>
         </is>
       </c>
-      <c r="E21" s="13" t="inlineStr">
+      <c r="E21" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1948,14 +2219,14 @@
           <t>ZN21</t>
         </is>
       </c>
-      <c r="E22" s="13" t="inlineStr">
+      <c r="E22" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -1980,14 +2251,14 @@
           <t>ZN22</t>
         </is>
       </c>
-      <c r="E23" s="12" t="inlineStr">
+      <c r="E23" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2012,14 +2283,14 @@
           <t>ZN23</t>
         </is>
       </c>
-      <c r="E24" s="13" t="inlineStr">
+      <c r="E24" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2044,14 +2315,14 @@
           <t>ZN24</t>
         </is>
       </c>
-      <c r="E25" s="13" t="inlineStr">
+      <c r="E25" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2076,14 +2347,14 @@
           <t>ZN25</t>
         </is>
       </c>
-      <c r="E26" s="13" t="inlineStr">
+      <c r="E26" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2108,14 +2379,14 @@
           <t>ZN26</t>
         </is>
       </c>
-      <c r="E27" s="13" t="inlineStr">
+      <c r="E27" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2140,14 +2411,14 @@
           <t>ZN27</t>
         </is>
       </c>
-      <c r="E28" s="12" t="inlineStr">
+      <c r="E28" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2172,14 +2443,14 @@
           <t>ZN28</t>
         </is>
       </c>
-      <c r="E29" s="13" t="inlineStr">
+      <c r="E29" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2204,14 +2475,14 @@
           <t>ZN29</t>
         </is>
       </c>
-      <c r="E30" s="13" t="inlineStr">
+      <c r="E30" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2236,14 +2507,14 @@
           <t>ZN30</t>
         </is>
       </c>
-      <c r="E31" s="13" t="inlineStr">
+      <c r="E31" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2268,14 +2539,14 @@
           <t>ZN31</t>
         </is>
       </c>
-      <c r="E32" s="13" t="inlineStr">
+      <c r="E32" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
@@ -2292,8 +2563,8 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -2336,7 +2607,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -2354,7 +2625,7 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2368,7 +2639,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
@@ -2386,7 +2657,7 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
@@ -2400,7 +2671,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
@@ -2418,7 +2689,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2432,7 +2703,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
@@ -2450,7 +2721,7 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2464,7 +2735,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
@@ -2482,7 +2753,7 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
@@ -2496,7 +2767,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -2514,7 +2785,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2528,7 +2799,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -2546,7 +2817,7 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E8" s="5" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2560,7 +2831,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
@@ -2578,7 +2849,7 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E9" s="4" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
@@ -2592,7 +2863,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
@@ -2610,7 +2881,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E10" s="5" t="inlineStr">
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2624,7 +2895,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
@@ -2642,21 +2913,21 @@
           <t>AZ1</t>
         </is>
       </c>
-      <c r="E11" s="12" t="inlineStr">
+      <c r="E11" s="11" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
@@ -2674,21 +2945,21 @@
           <t>AZ2</t>
         </is>
       </c>
-      <c r="E12" s="13" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 1</t>
+          <t>יחידה 199</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
@@ -2706,7 +2977,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E13" s="7" t="inlineStr">
+      <c r="E13" s="4" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2720,7 +2991,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>יחידה 777</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -2738,7 +3009,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E14" s="7" t="inlineStr">
+      <c r="E14" s="4" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2752,7 +3023,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>יחידה 777</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
@@ -2770,7 +3041,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E15" s="7" t="inlineStr">
+      <c r="E15" s="4" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2784,7 +3055,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>יחידה 777</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
@@ -2802,7 +3073,7 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E16" s="7" t="inlineStr">
+      <c r="E16" s="4" t="inlineStr">
         <is>
           <t>עובד</t>
         </is>
@@ -2816,7 +3087,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>תק"ש מספר 2</t>
+          <t>יחידה 777</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
@@ -2834,14 +3105,14 @@
           <t>AZ3</t>
         </is>
       </c>
-      <c r="E17" s="13" t="inlineStr">
+      <c r="E17" s="12" t="inlineStr">
         <is>
           <t>לא עובד</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>17/10/2021, 16:43:42</t>
+          <t>20/10/2021, 17:09:56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finish build the json database and fix some bugs
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:10:02</t>
+          <t>21/10/2021, 11:29:41</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:10:02</t>
+          <t>21/10/2021, 11:29:41</t>
         </is>
       </c>
     </row>
@@ -625,7 +625,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:10:02</t>
+          <t>21/10/2021, 11:29:41</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:10:02</t>
+          <t>21/10/2021, 11:29:41</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:10:02</t>
+          <t>21/10/2021, 11:29:41</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:10:02</t>
+          <t>21/10/2021, 11:29:41</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -872,7 +872,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -936,7 +936,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:54</t>
+          <t>21/10/2021, 11:29:24</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2098,7 +2098,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2258,7 +2258,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2386,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:30</t>
         </is>
       </c>
     </row>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:13</t>
         </is>
       </c>
     </row>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:13</t>
         </is>
       </c>
     </row>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>20/10/2021, 17:09:56</t>
+          <t>21/10/2021, 11:29:13</t>
         </is>
       </c>
     </row>

</xml_diff>